<commit_message>
updated final output to include missing Generation Charges
</commit_message>
<xml_diff>
--- a/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
+++ b/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
@@ -662,7 +662,11 @@
           <t>8.1438</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>8.3750</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>Feb-2023</t>
@@ -688,7 +692,11 @@
           <t>0.4309</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>8.3750</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>Feb-2023</t>
@@ -1466,7 +1474,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>13.2507</t>
+          <t>13.1332</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1496,7 +1504,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>13.2507</t>
+          <t>13.1332</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1802,7 +1810,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>6.3097</t>
+          <t>6.1922</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1832,7 +1840,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>6.3097</t>
+          <t>6.1922</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1942,7 +1950,11 @@
           <t>7.8909</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>7.3430</t>
+        </is>
+      </c>
       <c r="E52" t="inlineStr">
         <is>
           <t>Jan-2023</t>
@@ -1968,7 +1980,11 @@
           <t>6.9303</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>7.3430</t>
+        </is>
+      </c>
       <c r="E53" t="inlineStr">
         <is>
           <t>Jan-2023</t>
@@ -1996,7 +2012,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>5.9251</t>
+          <t>5.8076</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2026,7 +2042,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>5.9251</t>
+          <t>5.8076</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2348,7 +2364,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>5.3552</t>
+          <t>5.2377</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2378,7 +2394,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>5.3552</t>
+          <t>5.2377</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2572,7 +2588,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>5.7821</t>
+          <t>5.6646</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2602,7 +2618,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>5.7821</t>
+          <t>5.6646</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3044,7 +3060,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>6.3229</t>
+          <t>6.2054</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3074,7 +3090,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>6.3229</t>
+          <t>6.2054</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -3976,7 +3992,11 @@
           <t>7.6497</t>
         </is>
       </c>
-      <c r="D123" t="inlineStr"/>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>8.2890</t>
+        </is>
+      </c>
       <c r="E123" t="inlineStr">
         <is>
           <t>Mar-2023</t>
@@ -4002,7 +4022,11 @@
           <t>1.4492</t>
         </is>
       </c>
-      <c r="D124" t="inlineStr"/>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>8.2890</t>
+        </is>
+      </c>
       <c r="E124" t="inlineStr">
         <is>
           <t>Mar-2023</t>

</xml_diff>

<commit_message>
fixed missing Generation Charges for June and July 2024
</commit_message>
<xml_diff>
--- a/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
+++ b/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
@@ -1652,7 +1652,11 @@
           <t>5.4089</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>7.3862</t>
+        </is>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
           <t>Nov-2023</t>
@@ -1678,7 +1682,11 @@
           <t>9.4576</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>7.3862</t>
+        </is>
+      </c>
       <c r="E42" t="inlineStr">
         <is>
           <t>Nov-2023</t>
@@ -1704,7 +1712,11 @@
           <t>6.0079</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>5.6784</t>
+        </is>
+      </c>
       <c r="E43" t="inlineStr">
         <is>
           <t>Apr-2024</t>
@@ -1730,7 +1742,11 @@
           <t>3.8367</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>5.6784</t>
+        </is>
+      </c>
       <c r="E44" t="inlineStr">
         <is>
           <t>Apr-2024</t>
@@ -1756,7 +1772,11 @@
           <t>5.8154</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>6.1687</t>
+        </is>
+      </c>
       <c r="E45" t="inlineStr">
         <is>
           <t>Dec-2023</t>
@@ -1782,7 +1802,11 @@
           <t>75.9336</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>6.1687</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr">
         <is>
           <t>Dec-2023</t>
@@ -1898,7 +1922,11 @@
           <t>6.0997</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>7.1997</t>
+        </is>
+      </c>
       <c r="E50" t="inlineStr">
         <is>
           <t>Jul-2024</t>
@@ -1924,7 +1952,11 @@
           <t>20.1638</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>7.1997</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
           <t>Jul-2024</t>
@@ -2310,7 +2342,11 @@
           <t>6.8696</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>7.5218</t>
+        </is>
+      </c>
       <c r="E64" t="inlineStr">
         <is>
           <t>May-2023</t>
@@ -2336,7 +2372,11 @@
           <t>(18.8433)</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>7.5218</t>
+        </is>
+      </c>
       <c r="E65" t="inlineStr">
         <is>
           <t>May-2023</t>
@@ -2482,7 +2522,11 @@
           <t>6.9790</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>7.5979</t>
+        </is>
+      </c>
       <c r="E70" t="inlineStr">
         <is>
           <t>Apr-2023</t>
@@ -2508,7 +2552,11 @@
           <t>(7.7848)</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>7.5979</t>
+        </is>
+      </c>
       <c r="E71" t="inlineStr">
         <is>
           <t>Apr-2023</t>
@@ -2534,7 +2582,11 @@
           <t>5.9327</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>6.5110</t>
+        </is>
+      </c>
       <c r="E72" t="inlineStr">
         <is>
           <t>Aug-2023</t>
@@ -2560,7 +2612,11 @@
           <t>(49.3505)</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>6.5110</t>
+        </is>
+      </c>
       <c r="E73" t="inlineStr">
         <is>
           <t>Aug-2023</t>
@@ -2796,7 +2852,11 @@
           <t>6.2041</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>6.3620</t>
+        </is>
+      </c>
       <c r="E81" t="inlineStr">
         <is>
           <t>Mar-2024</t>
@@ -2822,7 +2882,11 @@
           <t>8.1576</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>6.3620</t>
+        </is>
+      </c>
       <c r="E82" t="inlineStr">
         <is>
           <t>Mar-2024</t>
@@ -3388,7 +3452,11 @@
           <t>6.0905</t>
         </is>
       </c>
-      <c r="D101" t="inlineStr"/>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>6.3987</t>
+        </is>
+      </c>
       <c r="E101" t="inlineStr">
         <is>
           <t>May-2024</t>
@@ -3414,7 +3482,11 @@
           <t>11.1399</t>
         </is>
       </c>
-      <c r="D102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>6.3987</t>
+        </is>
+      </c>
       <c r="E102" t="inlineStr">
         <is>
           <t>May-2024</t>
@@ -3440,7 +3512,11 @@
           <t>6.0476</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr"/>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>6.3784</t>
+        </is>
+      </c>
       <c r="E103" t="inlineStr">
         <is>
           <t>Sep-2023</t>
@@ -3466,7 +3542,11 @@
           <t>12.4009</t>
         </is>
       </c>
-      <c r="D104" t="inlineStr"/>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>6.3784</t>
+        </is>
+      </c>
       <c r="E104" t="inlineStr">
         <is>
           <t>Sep-2023</t>
@@ -3672,7 +3752,11 @@
           <t>6.0904</t>
         </is>
       </c>
-      <c r="D111" t="inlineStr"/>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>6.3361</t>
+        </is>
+      </c>
       <c r="E111" t="inlineStr">
         <is>
           <t>Feb-2024</t>
@@ -3698,7 +3782,11 @@
           <t>(23.2214)</t>
         </is>
       </c>
-      <c r="D112" t="inlineStr"/>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>6.3361</t>
+        </is>
+      </c>
       <c r="E112" t="inlineStr">
         <is>
           <t>Feb-2024</t>
@@ -3724,7 +3812,11 @@
           <t>5.9403</t>
         </is>
       </c>
-      <c r="D113" t="inlineStr"/>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>6.7152</t>
+        </is>
+      </c>
       <c r="E113" t="inlineStr">
         <is>
           <t>Jun-2024</t>
@@ -3750,7 +3842,11 @@
           <t>13.9284</t>
         </is>
       </c>
-      <c r="D114" t="inlineStr"/>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>6.7152</t>
+        </is>
+      </c>
       <c r="E114" t="inlineStr">
         <is>
           <t>Jun-2024</t>
@@ -3776,7 +3872,11 @@
           <t>6.4039</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr"/>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>7.1456</t>
+        </is>
+      </c>
       <c r="E115" t="inlineStr">
         <is>
           <t>Jun-2023</t>
@@ -3802,7 +3902,11 @@
           <t>(38.1362)</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr"/>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>7.1456</t>
+        </is>
+      </c>
       <c r="E116" t="inlineStr">
         <is>
           <t>Jun-2023</t>
@@ -3858,7 +3962,11 @@
           <t>6.1554</t>
         </is>
       </c>
-      <c r="D118" t="inlineStr"/>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>7.0155</t>
+        </is>
+      </c>
       <c r="E118" t="inlineStr">
         <is>
           <t>Jul-2023</t>
@@ -3884,7 +3992,11 @@
           <t>(32.2679)</t>
         </is>
       </c>
-      <c r="D119" t="inlineStr"/>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>7.0155</t>
+        </is>
+      </c>
       <c r="E119" t="inlineStr">
         <is>
           <t>Jul-2023</t>
@@ -3940,7 +4052,11 @@
           <t>5.7981</t>
         </is>
       </c>
-      <c r="D121" t="inlineStr"/>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>7.0722</t>
+        </is>
+      </c>
       <c r="E121" t="inlineStr">
         <is>
           <t>Oct-2023</t>
@@ -3966,7 +4082,11 @@
           <t>18.0214</t>
         </is>
       </c>
-      <c r="D122" t="inlineStr"/>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>7.0722</t>
+        </is>
+      </c>
       <c r="E122" t="inlineStr">
         <is>
           <t>Oct-2023</t>
@@ -4052,7 +4172,11 @@
           <t>6.0845</t>
         </is>
       </c>
-      <c r="D125" t="inlineStr"/>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>6.4921</t>
+        </is>
+      </c>
       <c r="E125" t="inlineStr">
         <is>
           <t>Jan-2024</t>
@@ -4078,7 +4202,11 @@
           <t>(28.2994)</t>
         </is>
       </c>
-      <c r="D126" t="inlineStr"/>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>6.4921</t>
+        </is>
+      </c>
       <c r="E126" t="inlineStr">
         <is>
           <t>Jan-2024</t>

</xml_diff>

<commit_message>
fixed negative Average Generation Cost
</commit_message>
<xml_diff>
--- a/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
+++ b/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8.2662</t>
+          <t>8877900</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3.5367</t>
+          <t>-1,171,489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>11.3173</t>
+          <t>10655000</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6.6169</t>
+          <t>-2,153,608</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.8026</t>
+          <t>2341709</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9605</t>
+          <t>1067489</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>8.1438</t>
+          <t>7877743</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.4309</t>
+          <t>-743,660</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -719,7 +719,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>4.8451</t>
+          <t>7916000</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.7673</t>
+          <t>-609,227</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5.2595</t>
+          <t>2702614</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6.0340</t>
+          <t>3875000</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.9382</t>
+          <t>-809,120.84</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>10.8191</t>
+          <t>8642400</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.7711</t>
+          <t>-797,421</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.8826</t>
+          <t>195267</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>5.3119</t>
+          <t>3049800</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6.4580</t>
+          <t>3875000</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.7218</t>
+          <t>-498,499.00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0898</t>
+          <t>410230</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>5.3218</t>
+          <t>2597056</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7.8135</t>
+          <t>349174.79</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>4.8382</t>
+          <t>3123227</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>(0.8065)</t>
+          <t>-217,343</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>5.0152</t>
+          <t>4538594</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>8.2548</t>
+          <t>3658652</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>4.9719</t>
+          <t>2815000</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>5.5496</t>
+          <t>1989216</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1319,7 +1319,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>5.8369</t>
+          <t>1200000</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>(2.3341)</t>
+          <t>-265,168.51</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>5.1956</t>
+          <t>2935250</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>5.8853</t>
+          <t>3875000</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>(4.9243)</t>
+          <t>-334,388.47</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11.2981</t>
+          <t>10908000</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>5.2365</t>
+          <t>-2,808,391</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>4.7313</t>
+          <t>3654000</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>4.1272</t>
+          <t>518267</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>4.5509</t>
+          <t>8003000</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>7.4017</t>
+          <t>-543,517</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>5.4089</t>
+          <t>4581683</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>9.4576</t>
+          <t>4883189</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>6.0079</t>
+          <t>7477405</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1739,7 +1739,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>3.8367</t>
+          <t>1119911</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>5.8154</t>
+          <t>9341370</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>75.9336</t>
+          <t>50000</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>6.4483</t>
+          <t>5555404</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>6.1999</t>
+          <t>-202,725</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1889,7 +1889,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10.9216</t>
+          <t>59558</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>6.0997</t>
+          <t>9618950</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>20.1638</t>
+          <t>1144646</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>7.8909</t>
+          <t>8271571</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2009,7 +2009,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>6.9303</t>
+          <t>-832,076</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>5.9085</t>
+          <t>9308500</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>5.1385</t>
+          <t>-1,164,230</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>4.7512</t>
+          <t>2565237</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>(0.9414)</t>
+          <t>1031718</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>5.3067</t>
+          <t>2157646</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2.8141</t>
+          <t>-209,588.65</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>4.8281</t>
+          <t>3578000</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2.0201</t>
+          <t>559750</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>5.2532</t>
+          <t>8559073</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>0.8278</t>
+          <t>-362,081</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>6.8696</t>
+          <t>9068364</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>(18.8433)</t>
+          <t>-302,037</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>4.9600</t>
+          <t>9716000</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2.8192</t>
+          <t>-1,827,635</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>4.8994</t>
+          <t>2984290</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>3.6974</t>
+          <t>1146720</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2519,7 +2519,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>6.9790</t>
+          <t>7512618</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>(7.7848)</t>
+          <t>-406,645</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>5.9327</t>
+          <t>8988115</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>(49.3505)</t>
+          <t>-101,097</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>5.9085</t>
+          <t>9015600</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>6.2415</t>
+          <t>-880,793</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2699,7 +2699,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>5.1417</t>
+          <t>7669000</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>(1.1973)</t>
+          <t>-420,420</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2759,7 +2759,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>5.1032</t>
+          <t>2910000</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2789,7 +2789,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>5.8866</t>
+          <t>3835000</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2819,7 +2819,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1.5674</t>
+          <t>-854,756.28</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>6.2041</t>
+          <t>7564710</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2879,7 +2879,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>8.1576</t>
+          <t>890495</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>4.8026</t>
+          <t>2341709</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.9605</t>
+          <t>1067489</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1.6797</t>
+          <t>716766</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>5.4513</t>
+          <t>2566405</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>7.9952</t>
+          <t>-355,701.08</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>0.3143</t>
+          <t>610659</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3089,7 +3089,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>(0.2417)</t>
+          <t>770874</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>5.6647</t>
+          <t>9034316</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>(22.8655)</t>
+          <t>-227,127</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>5.0191</t>
+          <t>2005940</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>6.7117</t>
+          <t>2022726.25</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -3239,7 +3239,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>5.4544</t>
+          <t>7617826</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -3269,7 +3269,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>9.8971</t>
+          <t>998698</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>5.3886</t>
+          <t>8559073</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>8.6206</t>
+          <t>-266,458</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>5.2331</t>
+          <t>2586392</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>6.3303</t>
+          <t>-288,097.09</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>(0.9588)</t>
+          <t>332421</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3449,7 +3449,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>6.0905</t>
+          <t>9367993</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11.1399</t>
+          <t>679365</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>6.0476</t>
+          <t>9048030</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3539,7 +3539,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>12.4009</t>
+          <t>561896</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>5.1989</t>
+          <t>1528060</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>6.1437</t>
+          <t>3500000</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>6.6913</t>
+          <t>637851.89</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>4.7785</t>
+          <t>2699527</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>5.0484</t>
+          <t>1528794</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>(0.8999)</t>
+          <t>175046</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3749,7 +3749,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>6.0904</t>
+          <t>9257235</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3779,7 +3779,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>(23.2214)</t>
+          <t>-90,640</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>5.9403</t>
+          <t>9591182</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3839,7 +3839,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>13.9284</t>
+          <t>1086733</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>6.4039</t>
+          <t>9562783</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3899,7 +3899,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>(38.1362)</t>
+          <t>-186,739</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3929,7 +3929,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>0.0187</t>
+          <t>369854</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>6.1554</t>
+          <t>9868300</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3989,7 +3989,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>(32.2679)</t>
+          <t>-254,900</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>3.7460</t>
+          <t>627848</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>5.7981</t>
+          <t>8581980</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>18.0214</t>
+          <t>1133295</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>7.6497</t>
+          <t>8544850</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>1.4492</t>
+          <t>-1,210,387</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>6.0845</t>
+          <t>8901698</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>(28.2994)</t>
+          <t>-115,253</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>5.4008</t>
+          <t>2713666</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4259,7 +4259,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>6.1199</t>
+          <t>3750000</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>2.2302</t>
+          <t>-393,470.05</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4319,7 +4319,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>4.7498</t>
+          <t>2448579</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>7.9329</t>
+          <t>1756860.50</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">

</xml_diff>

<commit_message>
fixed negative values in Average Generation Cost
</commit_message>
<xml_diff>
--- a/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
+++ b/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8877900</t>
+          <t>8.2662</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-1,171,489</t>
+          <t>3.5367</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>10655000</t>
+          <t>11.3173</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-2,153,608</t>
+          <t>6.6169</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2341709</t>
+          <t>4.8026</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1067489</t>
+          <t>0.9605</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7877743</t>
+          <t>8.1438</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>-743,660</t>
+          <t>0.4309</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -719,7 +719,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7916000</t>
+          <t>4.8451</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>-609,227</t>
+          <t>0.7673</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2702614</t>
+          <t>5.2595</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3875000</t>
+          <t>6.0340</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>-809,120.84</t>
+          <t>0.9382</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8642400</t>
+          <t>10.8191</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>-797,421</t>
+          <t>1.7711</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>195267</t>
+          <t>1.8826</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3049800</t>
+          <t>5.3119</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3875000</t>
+          <t>6.4580</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>-498,499.00</t>
+          <t>1.7218</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>410230</t>
+          <t>1.0898</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2597056</t>
+          <t>5.3218</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>349174.79</t>
+          <t>7.8135</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>3123227</t>
+          <t>4.8382</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>-217,343</t>
+          <t>-0.8065</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>4538594</t>
+          <t>5.0152</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>3658652</t>
+          <t>8.2548</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2815000</t>
+          <t>4.9719</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1989216</t>
+          <t>5.5496</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1319,7 +1319,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1200000</t>
+          <t>5.8369</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>-265,168.51</t>
+          <t>-2.3341</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2935250</t>
+          <t>5.1956</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>3875000</t>
+          <t>5.8853</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>-334,388.47</t>
+          <t>-4.9243</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10908000</t>
+          <t>11.2981</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>-2,808,391</t>
+          <t>5.2365</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3654000</t>
+          <t>4.7313</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>518267</t>
+          <t>4.1272</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>8003000</t>
+          <t>4.5509</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>-543,517</t>
+          <t>7.4017</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>4581683</t>
+          <t>5.4089</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>4883189</t>
+          <t>9.4576</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>7477405</t>
+          <t>6.0079</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1739,7 +1739,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1119911</t>
+          <t>3.8367</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>9341370</t>
+          <t>5.8154</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>50000</t>
+          <t>75.9336</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>5555404</t>
+          <t>6.4483</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>-202,725</t>
+          <t>6.1999</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1889,7 +1889,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>59558</t>
+          <t>10.9216</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>9618950</t>
+          <t>6.0997</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1144646</t>
+          <t>20.1638</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>8271571</t>
+          <t>7.8909</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2009,7 +2009,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>-832,076</t>
+          <t>6.9303</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>9308500</t>
+          <t>5.9085</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>-1,164,230</t>
+          <t>5.1385</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2565237</t>
+          <t>4.7512</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1031718</t>
+          <t>-0.9414</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2157646</t>
+          <t>5.3067</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>-209,588.65</t>
+          <t>2.8141</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>3578000</t>
+          <t>4.8281</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>559750</t>
+          <t>2.0201</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>8559073</t>
+          <t>5.2532</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>-362,081</t>
+          <t>0.8278</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>9068364</t>
+          <t>6.8696</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>-302,037</t>
+          <t>-18.8433</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>9716000</t>
+          <t>4.9600</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>-1,827,635</t>
+          <t>2.8192</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2984290</t>
+          <t>4.8994</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1146720</t>
+          <t>3.6974</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2519,7 +2519,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>7512618</t>
+          <t>6.9790</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>-406,645</t>
+          <t>-7.7848</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>8988115</t>
+          <t>5.9327</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>-101,097</t>
+          <t>-49.3505</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>9015600</t>
+          <t>5.9085</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>-880,793</t>
+          <t>6.2415</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2699,7 +2699,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>7669000</t>
+          <t>5.1417</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>-420,420</t>
+          <t>-1.1973</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2759,7 +2759,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2910000</t>
+          <t>5.1032</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2789,7 +2789,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>3835000</t>
+          <t>5.8866</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2819,7 +2819,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>-854,756.28</t>
+          <t>1.5674</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>7564710</t>
+          <t>6.2041</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2879,7 +2879,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>890495</t>
+          <t>8.1576</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2341709</t>
+          <t>4.8026</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>1067489</t>
+          <t>0.9605</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>716766</t>
+          <t>1.6797</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2566405</t>
+          <t>5.4513</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>-355,701.08</t>
+          <t>7.9952</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>610659</t>
+          <t>0.3143</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3089,7 +3089,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>770874</t>
+          <t>-0.2417</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>9034316</t>
+          <t>5.6647</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>-227,127</t>
+          <t>-22.8655</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2005940</t>
+          <t>5.0191</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2022726.25</t>
+          <t>6.7117</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -3239,7 +3239,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>7617826</t>
+          <t>5.4544</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -3269,7 +3269,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>998698</t>
+          <t>9.8971</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>8559073</t>
+          <t>5.3886</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>-266,458</t>
+          <t>8.6206</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>2586392</t>
+          <t>5.2331</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>-288,097.09</t>
+          <t>6.3303</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>332421</t>
+          <t>-0.9588</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3449,7 +3449,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>9367993</t>
+          <t>6.0905</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>679365</t>
+          <t>11.1399</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>9048030</t>
+          <t>6.0476</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3539,7 +3539,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>561896</t>
+          <t>12.4009</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>1528060</t>
+          <t>5.1989</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>3500000</t>
+          <t>6.1437</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>637851.89</t>
+          <t>6.6913</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>2699527</t>
+          <t>4.7785</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>1528794</t>
+          <t>5.0484</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>175046</t>
+          <t>-0.8999</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3749,7 +3749,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>9257235</t>
+          <t>6.0904</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3779,7 +3779,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>-90,640</t>
+          <t>-23.2214</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>9591182</t>
+          <t>5.9403</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3839,7 +3839,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>1086733</t>
+          <t>13.9284</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>9562783</t>
+          <t>6.4039</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3899,7 +3899,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>-186,739</t>
+          <t>-38.1362</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3929,7 +3929,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>369854</t>
+          <t>0.0187</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>9868300</t>
+          <t>6.1554</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3989,7 +3989,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>-254,900</t>
+          <t>-32.2679</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>627848</t>
+          <t>3.7460</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>8581980</t>
+          <t>5.7981</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>1133295</t>
+          <t>18.0214</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>8544850</t>
+          <t>7.6497</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>-1,210,387</t>
+          <t>1.4492</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>8901698</t>
+          <t>6.0845</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>-115,253</t>
+          <t>-28.2994</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>2713666</t>
+          <t>5.4008</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4259,7 +4259,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>3750000</t>
+          <t>6.1199</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>-393,470.05</t>
+          <t>2.2302</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4319,7 +4319,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>2448579</t>
+          <t>4.7498</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>1756860.50</t>
+          <t>7.9329</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">

</xml_diff>

<commit_message>
fixed date extraction from url
</commit_message>
<xml_diff>
--- a/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
+++ b/LEYECO IV/Historical_LEYECO_IV_GC_Breakdown.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -949,22 +949,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>47%</t>
+          <t>44%</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3049800</t>
+          <t>2909250</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>5.3119</t>
+          <t>5.6341</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6.1695</t>
+          <t>6.4217</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -979,7 +979,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -989,12 +989,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6.4580</t>
+          <t>6.6656</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6.1695</t>
+          <t>6.4217</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1009,22 +1009,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-8%</t>
+          <t>-3%</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>-498,499.00</t>
+          <t>-202,248.00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.7218</t>
+          <t>-3.9750</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6.1695</t>
+          <t>6.4217</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1189,167 +1189,167 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>43%</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4538594</t>
+          <t>2854500</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>5.0152</t>
+          <t>5.4550</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6.3914</t>
+          <t>6.1083</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Aug-2021</t>
+          <t>Nov-2018</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3658652</t>
+          <t>3750000</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>8.2548</t>
+          <t>6.5948</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6.3914</t>
+          <t>6.1083</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Aug-2021</t>
+          <t>Nov-2018</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>49%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2815000</t>
+          <t>110549.00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>4.9719</t>
+          <t>13.4062</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>5.6665</t>
+          <t>6.1083</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Jan-2018</t>
+          <t>Nov-2018</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>35%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1989216</t>
+          <t>4538594</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>5.5496</t>
+          <t>5.0152</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>5.6665</t>
+          <t>6.3914</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Jan-2018</t>
+          <t>Aug-2021</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>45%</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1200000</t>
+          <t>3658652</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>5.8369</t>
+          <t>8.2548</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5.6665</t>
+          <t>6.3914</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Jan-2018</t>
+          <t>Aug-2021</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-5%</t>
+          <t>49%</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>-265,168.51</t>
+          <t>2815000</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>-2.3341</t>
+          <t>4.9719</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1363,63 +1363,63 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>35%</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2935250</t>
+          <t>1989216</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>5.1956</t>
+          <t>5.5496</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>6.3319</t>
+          <t>5.6665</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>May-2018</t>
+          <t>Jan-2018</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>21%</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3875000</t>
+          <t>1200000</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>5.8853</t>
+          <t>5.8369</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>6.3319</t>
+          <t>5.6665</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>May-2018</t>
+          <t>Jan-2018</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1434,22 +1434,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>-334,388.47</t>
+          <t>-265,168.51</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>-4.9243</t>
+          <t>-2.3341</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>6.3319</t>
+          <t>5.6665</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>May-2018</t>
+          <t>Jan-2018</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1459,447 +1459,447 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>135%</t>
+          <t>45%</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>10908000</t>
+          <t>2935250</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11.2981</t>
+          <t>5.1956</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>13.1332</t>
+          <t>6.3319</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Sep-2022</t>
+          <t>May-2018</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-35%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>-2,808,391</t>
+          <t>3875000</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>5.2365</t>
+          <t>5.8853</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>13.1332</t>
+          <t>6.3319</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Sep-2022</t>
+          <t>May-2018</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>-5%</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3654000</t>
+          <t>-334,388.47</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>4.7313</t>
+          <t>-4.9243</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4.1092</t>
+          <t>6.3319</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Sep-2019</t>
+          <t>May-2018</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6%</t>
+          <t>115%</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>518267</t>
+          <t>9674500</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>4.1272</t>
+          <t>10.9885</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4.1092</t>
+          <t>11.7201</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Sep-2019</t>
+          <t>Jul-2022</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>107%</t>
+          <t>-15%</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>8003000</t>
+          <t>-1,251,678</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>4.5509</t>
+          <t>4.6046</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>4.1603</t>
+          <t>11.7201</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Feb-2021</t>
+          <t>Jul-2022</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-7%</t>
+          <t>45%</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>-543,517</t>
+          <t>3654000</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>7.4017</t>
+          <t>4.7313</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>4.1603</t>
+          <t>4.1092</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Feb-2021</t>
+          <t>Sep-2019</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>48.38%</t>
+          <t>6%</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4581683</t>
+          <t>518267</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>5.4089</t>
+          <t>4.1272</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7.3862</t>
+          <t>4.1092</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Nov-2023</t>
+          <t>Sep-2019</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>51.57%</t>
+          <t>123%</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4883189</t>
+          <t>10062000</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>9.4576</t>
+          <t>10.1460</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>7.3862</t>
+          <t>10.6794</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Nov-2023</t>
+          <t>Aug-2022</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>86.92%</t>
+          <t>-23%</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7477405</t>
+          <t>-1,899,587</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>6.0079</t>
+          <t>6.8360</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>5.6784</t>
+          <t>10.6794</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Apr-2024</t>
+          <t>Aug-2022</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>13.02%</t>
+          <t>107%</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>1119911</t>
+          <t>8003000</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>3.8367</t>
+          <t>4.5509</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5.6784</t>
+          <t>4.1603</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Apr-2024</t>
+          <t>Feb-2021</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>99.43%</t>
+          <t>-7%</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>9341370</t>
+          <t>-543,517</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>5.8154</t>
+          <t>7.4017</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>6.1687</t>
+          <t>4.1603</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Dec-2023</t>
+          <t>Feb-2021</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>0.53%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>50000</t>
+          <t>6784433</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>75.9336</t>
+          <t>8.3392</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>6.1687</t>
+          <t>9.1900</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Dec-2023</t>
+          <t>Apr-2022</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>104%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5555404</t>
+          <t>8070</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>6.4483</t>
+          <t>890.9646</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>6.1922</t>
+          <t>9.1900</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Aug-2022</t>
+          <t>Apr-2022</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-4%</t>
+          <t>48.38%</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>-202,725</t>
+          <t>4581683</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>6.1999</t>
+          <t>5.4089</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>6.1922</t>
+          <t>7.3862</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Aug-2022</t>
+          <t>Nov-2023</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>51.57%</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>59558</t>
+          <t>4883189</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10.9216</t>
+          <t>9.4576</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>4.0698</t>
+          <t>7.3862</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>May-2020</t>
+          <t>Nov-2023</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -1909,27 +1909,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>89.31%</t>
+          <t>86.92%</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>9618950</t>
+          <t>7477405</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>6.0997</t>
+          <t>6.0079</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>7.1997</t>
+          <t>5.6784</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Jul-2024</t>
+          <t>Apr-2024</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -1939,27 +1939,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>10.63%</t>
+          <t>13.02%</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1144646</t>
+          <t>1119911</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>20.1638</t>
+          <t>3.8367</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>7.1997</t>
+          <t>5.6784</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Jul-2024</t>
+          <t>Apr-2024</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -1969,27 +1969,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>111%</t>
+          <t>99.43%</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>8271571</t>
+          <t>9341370</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>7.8909</t>
+          <t>5.8154</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>7.3430</t>
+          <t>6.1687</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Jan-2023</t>
+          <t>Dec-2023</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -1999,27 +1999,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-11%</t>
+          <t>0.53%</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>-832,076</t>
+          <t>50000</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>6.9303</t>
+          <t>75.9336</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>7.3430</t>
+          <t>6.1687</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Jan-2023</t>
+          <t>Dec-2023</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2029,27 +2029,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>114%</t>
+          <t>61%</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>9308500</t>
+          <t>2644069</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>5.9085</t>
+          <t>7.7191</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>5.8076</t>
+          <t>7.6668</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Dec-2021</t>
+          <t>Feb-2022</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2059,27 +2059,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-14%</t>
+          <t>39%</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>-1,164,230</t>
+          <t>1661566</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>5.1385</t>
+          <t>8.2657</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>5.8076</t>
+          <t>7.6668</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Dec-2021</t>
+          <t>Feb-2022</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2089,57 +2089,57 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>35%</t>
+          <t>104%</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2565237</t>
+          <t>7123550</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>4.7512</t>
+          <t>8.7836</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3.6436</t>
+          <t>9.1422</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Aug-2019</t>
+          <t>Mar-2022</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>14%</t>
+          <t>-4%</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1031718</t>
+          <t>-241,188</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>-0.9414</t>
+          <t>-5.6830</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>3.6436</t>
+          <t>9.1422</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Aug-2019</t>
+          <t>Mar-2022</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2149,357 +2149,357 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>37%</t>
+          <t>1%</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2157646</t>
+          <t>59558</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>5.3067</t>
+          <t>10.9216</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>4.4809</t>
+          <t>4.0698</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Mar-2019</t>
+          <t>May-2020</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-4%</t>
+          <t>89.31%</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>-209,588.65</t>
+          <t>9618950</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2.8141</t>
+          <t>6.0997</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4.4809</t>
+          <t>7.1997</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Mar-2019</t>
+          <t>Jul-2024</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>10.63%</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>3578000</t>
+          <t>1144646</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>4.8281</t>
+          <t>20.1638</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>4.2472</t>
+          <t>7.1997</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Oct-2019</t>
+          <t>Jul-2024</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>111%</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>559750</t>
+          <t>8271571</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2.0201</t>
+          <t>7.8909</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>4.2472</t>
+          <t>7.3430</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Oct-2019</t>
+          <t>Jan-2023</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>104%</t>
+          <t>-11%</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8559073</t>
+          <t>-832,076</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>5.2532</t>
+          <t>6.9303</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>5.3612</t>
+          <t>7.3430</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>May-2021</t>
+          <t>Jan-2023</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-4%</t>
+          <t>114%</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>-362,081</t>
+          <t>9308500</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>0.8278</t>
+          <t>5.9085</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>5.3612</t>
+          <t>5.8076</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>May-2021</t>
+          <t>Dec-2021</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>103.42%</t>
+          <t>-14%</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>9068364</t>
+          <t>-1,164,230</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>6.8696</t>
+          <t>5.1385</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>7.5218</t>
+          <t>5.8076</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>May-2023</t>
+          <t>Dec-2021</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-3.44%</t>
+          <t>105%</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>-302,037</t>
+          <t>8879500</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>-18.8433</t>
+          <t>9.5341</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7.5218</t>
+          <t>10.3318</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>May-2023</t>
+          <t>Jun-2022</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>123%</t>
+          <t>-5%</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>9716000</t>
+          <t>-407,101</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>4.9600</t>
+          <t>-10.3300</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>5.2377</t>
+          <t>10.3318</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Oct-2021</t>
+          <t>Jun-2022</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-23%</t>
+          <t>42%</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>-1,827,635</t>
+          <t>2926000</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2.8192</t>
+          <t>5.3920</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>5.2377</t>
+          <t>5.9909</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Oct-2021</t>
+          <t>Sep-2018</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>38%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2984290</t>
+          <t>3875000</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>4.8994</t>
+          <t>6.7187</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>4.2786</t>
+          <t>5.9909</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Nov-2019</t>
+          <t>Sep-2018</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>15%</t>
+          <t>2%</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>1146720</t>
+          <t>153846.00</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>3.6974</t>
+          <t>3.4686</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4.2786</t>
+          <t>5.9909</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Nov-2019</t>
+          <t>Sep-2018</t>
         </is>
       </c>
       <c r="F69" t="n">
@@ -2509,57 +2509,57 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>105.70%</t>
+          <t>35%</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7512618</t>
+          <t>2565237</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>6.9790</t>
+          <t>4.7512</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>7.5979</t>
+          <t>3.6436</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Apr-2023</t>
+          <t>Aug-2019</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-5.72%</t>
+          <t>14%</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>-406,645</t>
+          <t>1031718</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>-7.7848</t>
+          <t>-0.9414</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>7.5979</t>
+          <t>3.6436</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Apr-2023</t>
+          <t>Aug-2019</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -2569,57 +2569,57 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>101.11%</t>
+          <t>37%</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8988115</t>
+          <t>2157646</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>5.9327</t>
+          <t>5.3067</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>6.5110</t>
+          <t>4.4809</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Aug-2023</t>
+          <t>Mar-2019</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-1.14%</t>
+          <t>-4%</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>-101,097</t>
+          <t>-209,588.65</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>-49.3505</t>
+          <t>2.8141</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>6.5110</t>
+          <t>4.4809</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Aug-2023</t>
+          <t>Mar-2019</t>
         </is>
       </c>
       <c r="F73" t="n">
@@ -2629,57 +2629,57 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>111%</t>
+          <t>45%</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9015600</t>
+          <t>3578000</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>5.9085</t>
+          <t>4.8281</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>5.6646</t>
+          <t>4.2472</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Nov-2021</t>
+          <t>Oct-2019</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-11%</t>
+          <t>7%</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>-880,793</t>
+          <t>559750</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>6.2415</t>
+          <t>2.0201</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>5.6646</t>
+          <t>4.2472</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Nov-2021</t>
+          <t>Oct-2019</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -2689,27 +2689,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>106%</t>
+          <t>104%</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7669000</t>
+          <t>8559073</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>5.1417</t>
+          <t>5.2532</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>5.4730</t>
+          <t>5.3612</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Apr-2021</t>
+          <t>May-2021</t>
         </is>
       </c>
       <c r="F76" t="n">
@@ -2719,27 +2719,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-6%</t>
+          <t>-4%</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>-420,420</t>
+          <t>-362,081</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>-1.1973</t>
+          <t>0.8278</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>5.4730</t>
+          <t>5.3612</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Apr-2021</t>
+          <t>May-2021</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -2749,207 +2749,207 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>49%</t>
+          <t>103.42%</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2910000</t>
+          <t>9068364</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>5.1032</t>
+          <t>6.8696</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>6.0392</t>
+          <t>7.5218</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Feb-2018</t>
+          <t>May-2023</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>-3.44%</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>3835000</t>
+          <t>-302,037</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>5.8866</t>
+          <t>-18.8433</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>6.0392</t>
+          <t>7.5218</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Feb-2018</t>
+          <t>May-2023</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-15%</t>
+          <t>123%</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>-854,756.28</t>
+          <t>9716000</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1.5674</t>
+          <t>4.9600</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>6.0392</t>
+          <t>5.2377</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Feb-2018</t>
+          <t>Oct-2021</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>89.42%</t>
+          <t>-23%</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7564710</t>
+          <t>-1,827,635</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>6.2041</t>
+          <t>2.8192</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6.3620</t>
+          <t>5.2377</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Mar-2024</t>
+          <t>Oct-2021</t>
         </is>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>10.53%</t>
+          <t>43%</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>890495</t>
+          <t>2924250</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>8.1576</t>
+          <t>5.4362</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6.3620</t>
+          <t>6.2006</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Mar-2024</t>
+          <t>Jul-2018</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>58%</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2341709</t>
+          <t>3875000</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>4.8026</t>
+          <t>6.1675</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>3.7636</t>
+          <t>6.2006</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Feb-2020</t>
+          <t>Jul-2018</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>15%</t>
+          <t>-1%</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>1067489</t>
+          <t>-70,976.00</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.9605</t>
+          <t>-9.3474</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>3.7636</t>
+          <t>6.2006</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Feb-2020</t>
+          <t>Jul-2018</t>
         </is>
       </c>
       <c r="F84" t="n">
@@ -2959,117 +2959,117 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>38%</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>716766</t>
+          <t>2984290</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1.6797</t>
+          <t>4.8994</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>3.8418</t>
+          <t>4.2786</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Nov-2020</t>
+          <t>Nov-2019</t>
         </is>
       </c>
       <c r="F85" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2566405</t>
+          <t>1146720</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>5.4513</t>
+          <t>3.6974</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>4.4388</t>
+          <t>4.2786</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Apr-2019</t>
+          <t>Nov-2019</t>
         </is>
       </c>
       <c r="F86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-6%</t>
+          <t>105.70%</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>-355,701.08</t>
+          <t>7512618</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>7.9952</t>
+          <t>6.9790</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>4.4388</t>
+          <t>7.5979</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Apr-2019</t>
+          <t>Apr-2023</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>8%</t>
+          <t>-5.72%</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>610659</t>
+          <t>-406,645</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>0.3143</t>
+          <t>-7.7848</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>3.6318</t>
+          <t>7.5979</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Jul-2020</t>
+          <t>Apr-2023</t>
         </is>
       </c>
       <c r="F88" t="n">
@@ -3079,327 +3079,327 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>101.11%</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>770874</t>
+          <t>8988115</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>-0.2417</t>
+          <t>5.9327</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>3.6579</t>
+          <t>6.5110</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Oct-2020</t>
+          <t>Aug-2023</t>
         </is>
       </c>
       <c r="F89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>103%</t>
+          <t>-1.14%</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>9034316</t>
+          <t>-101,097</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>5.6647</t>
+          <t>-49.3505</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>6.2054</t>
+          <t>6.5110</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Sep-2021</t>
+          <t>Aug-2023</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>-3%</t>
+          <t>111%</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>-227,127</t>
+          <t>9015600</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>-22.8655</t>
+          <t>5.9085</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>6.2054</t>
+          <t>5.6646</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Sep-2021</t>
+          <t>Nov-2021</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>-11%</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2005940</t>
+          <t>-880,793</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>5.0191</t>
+          <t>6.2415</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>5.0244</t>
+          <t>5.6646</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Jun-2019</t>
+          <t>Nov-2021</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>106%</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2022726.25</t>
+          <t>7669000</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>6.7117</t>
+          <t>5.1417</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>5.0244</t>
+          <t>5.4730</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Jun-2019</t>
+          <t>Apr-2021</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>-6%</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>7617826</t>
+          <t>-420,420</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>5.4544</t>
+          <t>-1.1973</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>5.8770</t>
+          <t>5.4730</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Jul-2021</t>
+          <t>Apr-2021</t>
         </is>
       </c>
       <c r="F94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>998698</t>
+          <t>7195440</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>9.8971</t>
+          <t>8.8735</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>5.8770</t>
+          <t>9.7075</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Jul-2021</t>
+          <t>May-2022</t>
         </is>
       </c>
       <c r="F95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>103%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>8559073</t>
+          <t>18672</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>5.3886</t>
+          <t>377.7270</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>5.1870</t>
+          <t>9.7075</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Jun-2021</t>
+          <t>May-2022</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>-3%</t>
+          <t>49%</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>-266,458</t>
+          <t>2910000</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>8.6206</t>
+          <t>5.1032</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>5.1870</t>
+          <t>6.0392</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Jun-2021</t>
+          <t>Feb-2018</t>
         </is>
       </c>
       <c r="F97" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>42%</t>
+          <t>65%</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2586392</t>
+          <t>3835000</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>5.2331</t>
+          <t>5.8866</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>4.5030</t>
+          <t>6.0392</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Feb-2019</t>
+          <t>Feb-2018</t>
         </is>
       </c>
       <c r="F98" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>-5%</t>
+          <t>-15%</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>-288,097.09</t>
+          <t>-854,756.28</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>6.3303</t>
+          <t>1.5674</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>4.5030</t>
+          <t>6.0392</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Feb-2019</t>
+          <t>Feb-2018</t>
         </is>
       </c>
       <c r="F99" t="n">
@@ -3409,147 +3409,147 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>4%</t>
+          <t>89.42%</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>332421</t>
+          <t>7564710</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>-0.9588</t>
+          <t>6.2041</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>3.7654</t>
+          <t>6.3620</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Jan-2021</t>
+          <t>Mar-2024</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>93.18%</t>
+          <t>10.53%</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>9367993</t>
+          <t>890495</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>6.0905</t>
+          <t>8.1576</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>6.3987</t>
+          <t>6.3620</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>May-2024</t>
+          <t>Mar-2024</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>6.76%</t>
+          <t>33%</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>679365</t>
+          <t>2341709</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11.1399</t>
+          <t>4.8026</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>6.3987</t>
+          <t>3.7636</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>May-2024</t>
+          <t>Feb-2020</t>
         </is>
       </c>
       <c r="F102" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>94.11%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>9048030</t>
+          <t>1067489</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>6.0476</t>
+          <t>0.9605</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>6.3784</t>
+          <t>3.7636</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Sep-2023</t>
+          <t>Feb-2020</t>
         </is>
       </c>
       <c r="F103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>5.84%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>561896</t>
+          <t>716766</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>12.4009</t>
+          <t>1.6797</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>6.3784</t>
+          <t>3.8418</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Sep-2023</t>
+          <t>Nov-2020</t>
         </is>
       </c>
       <c r="F104" t="n">
@@ -3559,27 +3559,27 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>27%</t>
+          <t>43%</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>1528060</t>
+          <t>2825500</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>5.1989</t>
+          <t>5.3728</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>6.1508</t>
+          <t>5.6836</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Apr-2018</t>
+          <t>Aug-2018</t>
         </is>
       </c>
       <c r="F105" t="n">
@@ -3589,27 +3589,27 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>62%</t>
+          <t>58%</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>3500000</t>
+          <t>3750000</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>6.1437</t>
+          <t>6.5320</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>6.1508</t>
+          <t>5.6836</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Apr-2018</t>
+          <t>Aug-2018</t>
         </is>
       </c>
       <c r="F106" t="n">
@@ -3619,27 +3619,27 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>11%</t>
+          <t>-1%</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>637851.89</t>
+          <t>-57,223.00</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>6.6913</t>
+          <t>33.9436</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>6.1508</t>
+          <t>5.6836</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Apr-2018</t>
+          <t>Aug-2018</t>
         </is>
       </c>
       <c r="F107" t="n">
@@ -3649,27 +3649,27 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>45%</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2699527</t>
+          <t>2566405</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>4.7785</t>
+          <t>5.4513</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>4.2460</t>
+          <t>4.4388</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Dec-2019</t>
+          <t>Apr-2019</t>
         </is>
       </c>
       <c r="F108" t="n">
@@ -3679,27 +3679,27 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>19%</t>
+          <t>-6%</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>1528794</t>
+          <t>-355,701.08</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>5.0484</t>
+          <t>7.9952</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>4.2460</t>
+          <t>4.4388</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Dec-2019</t>
+          <t>Apr-2019</t>
         </is>
       </c>
       <c r="F109" t="n">
@@ -3709,27 +3709,27 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2%</t>
+          <t>8%</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>175046</t>
+          <t>610659</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>-0.8999</t>
+          <t>0.3143</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>3.9712</t>
+          <t>3.6318</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Aug-2020</t>
+          <t>Jul-2020</t>
         </is>
       </c>
       <c r="F110" t="n">
@@ -3739,207 +3739,207 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>100.95%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>9257235</t>
+          <t>770874</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>6.0904</t>
+          <t>-0.2417</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>6.3361</t>
+          <t>3.6579</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Feb-2024</t>
+          <t>Oct-2020</t>
         </is>
       </c>
       <c r="F111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>-0.99%</t>
+          <t>103%</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>-90,640</t>
+          <t>9034316</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>-23.2214</t>
+          <t>5.6647</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>6.3361</t>
+          <t>6.2054</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Feb-2024</t>
+          <t>Sep-2021</t>
         </is>
       </c>
       <c r="F112" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>89.77%</t>
+          <t>-3%</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>9591182</t>
+          <t>-227,127</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>5.9403</t>
+          <t>-22.8655</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>6.7152</t>
+          <t>6.2054</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Jun-2024</t>
+          <t>Sep-2021</t>
         </is>
       </c>
       <c r="F113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>10.17%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>1086733</t>
+          <t>2005940</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>13.9284</t>
+          <t>5.0191</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>6.7152</t>
+          <t>5.0244</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Jun-2024</t>
+          <t>Jun-2019</t>
         </is>
       </c>
       <c r="F114" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>101.96%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>9562783</t>
+          <t>2022726.25</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>6.4039</t>
+          <t>6.7117</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>7.1456</t>
+          <t>5.0244</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Jun-2023</t>
+          <t>Jun-2019</t>
         </is>
       </c>
       <c r="F115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>-1.99%</t>
+          <t>135%</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>-186,739</t>
+          <t>10908000</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>-38.1362</t>
+          <t>11.2981</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>7.1456</t>
+          <t>13.1332</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Jun-2023</t>
+          <t>Sep-2022</t>
         </is>
       </c>
       <c r="F116" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>-35%</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>369854</t>
+          <t>-2,808,391</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>0.0187</t>
+          <t>5.2365</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>3.8807</t>
+          <t>13.1332</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Dec-2020</t>
+          <t>Sep-2022</t>
         </is>
       </c>
       <c r="F117" t="n">
@@ -3949,27 +3949,27 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>102.60%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>9868300</t>
+          <t>7617826</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>6.1554</t>
+          <t>5.4544</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>7.0155</t>
+          <t>5.8770</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Jul-2023</t>
+          <t>Jul-2021</t>
         </is>
       </c>
       <c r="F118" t="n">
@@ -3979,27 +3979,27 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>-2.65%</t>
+          <t>12%</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>-254,900</t>
+          <t>998698</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>-32.2679</t>
+          <t>9.8971</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>7.0155</t>
+          <t>5.8770</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Jul-2023</t>
+          <t>Jul-2021</t>
         </is>
       </c>
       <c r="F119" t="n">
@@ -4009,147 +4009,147 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>8%</t>
+          <t>103%</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>627848</t>
+          <t>8559073</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>3.7460</t>
+          <t>5.3886</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>3.9601</t>
+          <t>5.1870</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Jun-2020</t>
+          <t>Jun-2021</t>
         </is>
       </c>
       <c r="F120" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>88.29%</t>
+          <t>-3%</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>8581980</t>
+          <t>-266,458</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>5.7981</t>
+          <t>8.6206</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>7.0722</t>
+          <t>5.1870</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Oct-2023</t>
+          <t>Jun-2021</t>
         </is>
       </c>
       <c r="F121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11.66%</t>
+          <t>42%</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>1133295</t>
+          <t>2586392</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>18.0214</t>
+          <t>5.2331</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>7.0722</t>
+          <t>4.5030</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Oct-2023</t>
+          <t>Feb-2019</t>
         </is>
       </c>
       <c r="F122" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>116.49%</t>
+          <t>-5%</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>8544850</t>
+          <t>-288,097.09</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>7.6497</t>
+          <t>6.3303</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>8.2890</t>
+          <t>4.5030</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Mar-2023</t>
+          <t>Feb-2019</t>
         </is>
       </c>
       <c r="F123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>-16.50%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>-1,210,387</t>
+          <t>332421</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>1.4492</t>
+          <t>-0.9588</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>8.2890</t>
+          <t>3.7654</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Mar-2023</t>
+          <t>Jan-2021</t>
         </is>
       </c>
       <c r="F124" t="n">
@@ -4159,27 +4159,27 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>101.28%</t>
+          <t>93.18%</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>8901698</t>
+          <t>9367993</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>6.0845</t>
+          <t>6.0905</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>6.4921</t>
+          <t>6.3987</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Jan-2024</t>
+          <t>May-2024</t>
         </is>
       </c>
       <c r="F125" t="n">
@@ -4189,27 +4189,27 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>-1.31%</t>
+          <t>6.76%</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>-115,253</t>
+          <t>679365</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>-28.2994</t>
+          <t>11.1399</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>6.4921</t>
+          <t>6.3987</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Jan-2024</t>
+          <t>May-2024</t>
         </is>
       </c>
       <c r="F126" t="n">
@@ -4219,150 +4219,1110 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>94.11%</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2713666</t>
+          <t>9048030</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>5.4008</t>
+          <t>6.0476</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>5.9376</t>
+          <t>6.3784</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Jan-2019</t>
+          <t>Sep-2023</t>
         </is>
       </c>
       <c r="F127" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>62%</t>
+          <t>5.84%</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>3750000</t>
+          <t>561896</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>6.1199</t>
+          <t>12.4009</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>5.9376</t>
+          <t>6.3784</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Jan-2019</t>
+          <t>Sep-2023</t>
         </is>
       </c>
       <c r="F128" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>-6%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>-393,470.05</t>
+          <t>1528060</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>2.2302</t>
+          <t>5.1989</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>5.9376</t>
+          <t>6.1508</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Jan-2019</t>
+          <t>Apr-2018</t>
         </is>
       </c>
       <c r="F129" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>2448579</t>
+          <t>3500000</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>4.7498</t>
+          <t>6.1437</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>5.1095</t>
+          <t>6.1508</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Jul-2019</t>
+          <t>Apr-2018</t>
         </is>
       </c>
       <c r="F130" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
+          <t>11%</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>637851.89</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>6.6913</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>6.1508</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Apr-2018</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>33%</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>2699527</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>4.7785</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>4.2460</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Dec-2019</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>19%</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>1528794</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>5.0484</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>4.2460</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Dec-2019</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>175046</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>-0.8999</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>3.9712</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Aug-2020</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>100.95%</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>9257235</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>6.0904</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>6.3361</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Feb-2024</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>-0.99%</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>-90,640</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>-23.2214</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>6.3361</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Feb-2024</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>89.77%</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>9591182</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>5.9403</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>6.7152</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Jun-2024</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>10.17%</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>1086733</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>13.9284</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>6.7152</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Jun-2024</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>41%</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>2835000</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>5.2946</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>5.8861</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Jun-2018</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>55%</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>3750000</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>5.8125</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>5.8861</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Jun-2018</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>287627.00</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>8.4468</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>5.8861</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Jun-2018</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>101.96%</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>9562783</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>6.4039</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>7.1456</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Jun-2023</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>-1.99%</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>-186,739</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>-38.1362</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>7.1456</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Jun-2023</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>104%</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>5555404</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>6.4483</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>6.1922</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Jan-2022</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>-4%</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>-202,725</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>6.1999</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>6.1922</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Jan-2022</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>369854</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>0.0187</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>3.8807</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Dec-2020</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>102.60%</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>9868300</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>6.1554</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>7.0155</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Jul-2023</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>-2.65%</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>-254,900</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>-32.2679</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>7.0155</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Jul-2023</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>47%</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>3049800</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>5.3119</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>6.1695</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Dec-2018</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>60%</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>3875000</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>6.4580</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>6.1695</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Dec-2018</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>-8%</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>-498,499.00</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>1.7218</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>6.1695</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Dec-2018</t>
+        </is>
+      </c>
+      <c r="F151" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>627848</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>3.7460</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>3.9601</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Jun-2020</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>88.29%</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>8581980</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>5.7981</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>7.0722</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Oct-2023</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>11.66%</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>1133295</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>18.0214</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>7.0722</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Oct-2023</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>116.49%</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>8544850</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>7.6497</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>8.2890</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Mar-2023</t>
+        </is>
+      </c>
+      <c r="F155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>-16.50%</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>-1,210,387</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>1.4492</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>8.2890</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Mar-2023</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>101.28%</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>8901698</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>6.0845</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>6.4921</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Jan-2024</t>
+        </is>
+      </c>
+      <c r="F157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>-1.31%</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>-115,253</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>-28.2994</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>6.4921</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Jan-2024</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>45%</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>2713666</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>5.4008</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>5.9376</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Jan-2019</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>62%</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>3750000</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>6.1199</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>5.9376</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Jan-2019</t>
+        </is>
+      </c>
+      <c r="F160" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>-6%</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>-393,470.05</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>2.2302</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>5.9376</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Jan-2019</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>2448579</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>4.7498</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>5.1095</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Jul-2019</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
           <t>22%</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
+      <c r="B163" t="inlineStr">
         <is>
           <t>1756860.50</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
+      <c r="C163" t="inlineStr">
         <is>
           <t>7.9329</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr">
+      <c r="D163" t="inlineStr">
         <is>
           <t>5.1095</t>
         </is>
       </c>
-      <c r="E131" t="inlineStr">
+      <c r="E163" t="inlineStr">
         <is>
           <t>Jul-2019</t>
         </is>
       </c>
-      <c r="F131" t="n">
+      <c r="F163" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>